<commit_message>
inclusão de categorias de despesa e receita utilizadas nos lançamentos financeiros
</commit_message>
<xml_diff>
--- a/db/docs/lancamento_financeiro.xlsx
+++ b/db/docs/lancamento_financeiro.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="510" yWindow="555" windowWidth="15015" windowHeight="5835"/>
   </bookViews>
   <sheets>
-    <sheet name="Página1" sheetId="1" r:id="rId1"/>
+    <sheet name="lancamento_financeiro" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Página1!$A$1:$AA$532</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">lancamento_financeiro!$A$1:$AA$532</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -803,7 +803,7 @@
   <dimension ref="A1:P665"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>